<commit_message>
Cambios en el manejo de creacion de carpeta
</commit_message>
<xml_diff>
--- a/aDiary/template.xlsx
+++ b/aDiary/template.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">$replaceMe</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="2">
   <si>
     <t xml:space="preserve">$</t>
   </si>
@@ -125,10 +122,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -141,12 +138,38 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login y creacion basico implementado en conjunto con ManejoDatos
</commit_message>
<xml_diff>
--- a/aDiary/template.xlsx
+++ b/aDiary/template.xlsx
@@ -8,22 +8,19 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="2">
-  <si>
-    <t xml:space="preserve">$</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t xml:space="preserve">#end</t>
   </si>
@@ -35,12 +32,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -57,16 +53,105 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Mangal"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -74,8 +159,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -99,6 +199,22 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -106,14 +222,90 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Título" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -122,10 +314,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -137,48 +329,14 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>